<commit_message>
edit local file then commit
commit excel file to B2 branch
</commit_message>
<xml_diff>
--- a/ExcelT1.xlsx
+++ b/ExcelT1.xlsx
@@ -349,27 +349,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>